<commit_message>
Connecting download to update to Redis
</commit_message>
<xml_diff>
--- a/PIM.xlsx
+++ b/PIM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17031"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17114"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,18 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" r:id="rId1"/>
-    <sheet name="LoV" sheetId="2" r:id="rId2"/>
-    <sheet name="Insurance" sheetId="3" r:id="rId3"/>
-    <sheet name="Web Access" sheetId="4" r:id="rId4"/>
-    <sheet name="PII" sheetId="5" r:id="rId5"/>
+    <sheet name="Insurance" sheetId="3" r:id="rId2"/>
+    <sheet name="PII" sheetId="5" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Web Access'!$J$1:$M$54</definedName>
-  </definedNames>
   <calcPr calcId="171026" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="342">
   <si>
     <t>belongs</t>
   </si>
@@ -882,36 +877,6 @@
     <t>vaidya.emirates.travel</t>
   </si>
   <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>Credit Card</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>Debit Card</t>
-  </si>
-  <si>
-    <t>LC</t>
-  </si>
-  <si>
-    <t>SA</t>
-  </si>
-  <si>
-    <t>LA</t>
-  </si>
-  <si>
-    <t>LI</t>
-  </si>
-  <si>
-    <t>GI</t>
-  </si>
-  <si>
-    <t>CL</t>
-  </si>
-  <si>
     <t>Policy Number</t>
   </si>
   <si>
@@ -1062,229 +1027,16 @@
     <t>Home</t>
   </si>
   <si>
-    <t>Account_Number</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>Unique_Number</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t>Valid_From</t>
   </si>
   <si>
     <t>Valid_To</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Customer_Service_Number</t>
-  </si>
-  <si>
-    <t>Web_Access</t>
-  </si>
-  <si>
-    <t>UID</t>
-  </si>
-  <si>
-    <t>PWD</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Search</t>
-  </si>
-  <si>
-    <t>WA</t>
-  </si>
-  <si>
-    <t>Evernote Note taking app</t>
-  </si>
-  <si>
-    <t>Evernote</t>
-  </si>
-  <si>
-    <t>UnV4*RBq</t>
-  </si>
-  <si>
-    <t>8mVzgbqe</t>
-  </si>
-  <si>
-    <t>ICICI Txn Pwd</t>
-  </si>
-  <si>
-    <t>TStd</t>
-  </si>
-  <si>
-    <t>T8mVzgbqe</t>
-  </si>
-  <si>
-    <t>Face Book</t>
-  </si>
-  <si>
-    <t>Amazon</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/ap/signin?_encoding=UTF8&amp;amp;openid.assoc_handle=usflex&amp;amp;openid.return_to=https%3A%2F%2Fwww.amazon.com%2Fgp%2Fcss%2Fshiptrack%2Fview.html%3Fie%3DUTF8%26addressID%3Djhrlkupop%26trackingNumber%3D1ZA50W201345143658%26latestArrivalDate%3D1295582400%26shipMethod%3DUPS_NEXT_SAVER_COM%26orderID%3D102-3555103-6389809%26ref%3D%26shipmentDate%3D1295478379%26carrierId%3DUPS&amp;amp;openid.mode=checkid_setup&amp;amp;openid.ns=http%3A%2F%2Fspecs.openid.net%2Fauth%2F2.0&amp;amp;openid.claimed_id=http%3A%2F%2Fspecs.openid.net%2Fauth%2F2.0%2Fidentifier_select&amp;amp;openid.pape.max_auth_age=900&amp;amp;openid.ns.pape=http%3A%2F%2Fspecs.openid.net%2Fextensions%2Fpape%2F1.0&amp;amp;openid.identity=http%3A%2F%2Fspecs.openid.net%2Fauth%2F2.0%2Fidentifier_select</t>
-  </si>
-  <si>
-    <t>Pay Phrease : Dark Black Platinum / 7571</t>
-  </si>
-  <si>
-    <t>Railways</t>
-  </si>
-  <si>
-    <t>Membership # : 251790</t>
-  </si>
-  <si>
-    <t>Bajaj Allianz</t>
-  </si>
-  <si>
-    <t>bajajallianz.com</t>
-  </si>
-  <si>
-    <t>Rpv1971Rpv</t>
-  </si>
-  <si>
-    <t>book.goindigo.in</t>
-  </si>
-  <si>
-    <t>google.com</t>
-  </si>
-  <si>
-    <t>Linked In</t>
-  </si>
-  <si>
-    <t>linkedin.com</t>
-  </si>
-  <si>
-    <t>maavaishnodevi.org</t>
-  </si>
-  <si>
-    <t>eBay India</t>
-  </si>
-  <si>
-    <t>ted.com</t>
-  </si>
-  <si>
-    <t>Office Insurance</t>
-  </si>
-  <si>
-    <t>uhcindia.com</t>
-  </si>
-  <si>
-    <t>Apple Store</t>
-  </si>
-  <si>
-    <t>store.apple.com</t>
-  </si>
-  <si>
-    <t>Ilhswmwa24x7</t>
-  </si>
-  <si>
-    <t>eSeva</t>
-  </si>
-  <si>
-    <t>uttaradimath.org</t>
-  </si>
-  <si>
-    <t>T[b662082</t>
-  </si>
-  <si>
-    <t>IncomeTax</t>
-  </si>
-  <si>
-    <t>vrllogistics.in</t>
-  </si>
-  <si>
-    <t>Anita</t>
-  </si>
-  <si>
-    <t>Union Bank of India</t>
-  </si>
-  <si>
-    <t>UBI</t>
-  </si>
-  <si>
-    <t>TStd 2</t>
-  </si>
-  <si>
-    <t>TUnV4*RBq</t>
-  </si>
-  <si>
-    <t>India Times Shopping</t>
-  </si>
-  <si>
-    <t>Jasmine Adda</t>
-  </si>
-  <si>
-    <t>Microsoft Sky Drive</t>
-  </si>
-  <si>
-    <t>opensubtitles.org</t>
-  </si>
-  <si>
-    <t>Wolfram</t>
-  </si>
-  <si>
-    <t>Unit Trust of India</t>
-  </si>
-  <si>
-    <t>UTI Vaidya</t>
-  </si>
-  <si>
-    <t>https://www.utimf.com/_login/utilogin.aspx</t>
-  </si>
-  <si>
-    <t>Git Hub</t>
-  </si>
-  <si>
-    <t>My Universe</t>
-  </si>
-  <si>
-    <t>UnV45RBq</t>
-  </si>
-  <si>
-    <t>IDFC</t>
-  </si>
-  <si>
-    <t>Packet Pub</t>
-  </si>
-  <si>
-    <t>Think Vidya</t>
-  </si>
-  <si>
-    <t>delyver.com</t>
-  </si>
-  <si>
-    <t>Ilhswmwa24$7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Edumerge </t>
-  </si>
-  <si>
-    <t>Edumerge : Amogh School</t>
-  </si>
-  <si>
-    <t>MY CAMS</t>
-  </si>
-  <si>
-    <t>My CAMS</t>
-  </si>
-  <si>
-    <t>HDFC Home Insurance</t>
-  </si>
-  <si>
-    <t>Safari books online - GE</t>
-  </si>
-  <si>
-    <t>Unique_Number</t>
   </si>
   <si>
     <t>Aadhar</t>
@@ -1516,57 +1268,57 @@
     </xf>
   </cellXfs>
   <cellStyles count="53">
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1910,7 +1662,7 @@
   </sheetPr>
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="128" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="128" workbookViewId="0">
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
@@ -4097,78 +3849,9 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>192</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr autoPageBreaks="0"/>
-  </sheetPr>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -4185,31 +3868,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4223,22 +3906,22 @@
         <v>168</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="G2" s="12">
         <v>38308</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -4246,16 +3929,16 @@
         <v>616323370</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C3" s="8">
         <v>185</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F3" s="9">
         <v>42042</v>
@@ -4264,10 +3947,10 @@
         <v>47855</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4275,16 +3958,16 @@
         <v>616323371</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C4" s="8">
         <v>184</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F4" s="9">
         <v>42042</v>
@@ -4293,10 +3976,10 @@
         <v>25034</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4304,28 +3987,28 @@
         <v>610182022</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C5" s="8">
         <v>14</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="G5" s="12">
         <v>584.29999999999995</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -4333,28 +4016,28 @@
         <v>614562537</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C6" s="8">
         <v>149</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="G6" s="12">
         <v>8759</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -4362,28 +4045,28 @@
         <v>617350468</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C7" s="8">
         <v>818</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4391,28 +4074,28 @@
         <v>360295953</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C8" s="8">
         <v>93</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="G8" s="12">
         <v>5182</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -4420,28 +4103,28 @@
         <v>360444421</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C9" s="8">
         <v>14</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="G9" s="12">
         <v>5970</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -4449,28 +4132,28 @@
         <v>720226528</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C10" s="8">
         <v>27</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="G10" s="12">
         <v>3028</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -4478,28 +4161,28 @@
         <v>612539751</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="C11" s="8">
         <v>122</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="G11" s="12">
         <v>9941</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -4507,28 +4190,28 @@
         <v>612350047</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C12" s="8">
         <v>88</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="G12" s="12">
         <v>4202</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -4542,22 +4225,22 @@
         <v>14</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="G13" s="12">
         <v>1249</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4565,28 +4248,28 @@
         <v>615668468</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C14" s="8">
         <v>178</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -4594,28 +4277,28 @@
         <v>648434072</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C15" s="8">
         <v>149</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G15" s="12">
         <v>10267</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -4623,28 +4306,28 @@
         <v>648434073</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C16" s="8">
         <v>149</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G16" s="12">
         <v>9802</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -4652,28 +4335,28 @@
         <v>648434071</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C17" s="8">
         <v>149</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G17" s="12">
         <v>10752</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -4681,28 +4364,28 @@
         <v>648434070</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C18" s="8">
         <v>149</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G18" s="12">
         <v>11331</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -4710,28 +4393,28 @@
         <v>648434069</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C19" s="8">
         <v>149</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G19" s="12">
         <v>11964</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -4739,28 +4422,28 @@
         <v>648434068</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C20" s="8">
         <v>149</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G20" s="12">
         <v>12655</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -4768,28 +4451,28 @@
         <v>648434067</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C21" s="8">
         <v>149</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G21" s="12">
         <v>13406</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -4797,28 +4480,28 @@
         <v>648434066</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C22" s="8">
         <v>149</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G22" s="12">
         <v>13904</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -4826,28 +4509,28 @@
         <v>648434065</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C23" s="8">
         <v>149</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G23" s="12">
         <v>14789</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -4855,28 +4538,28 @@
         <v>648434064</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C24" s="8">
         <v>149</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G24" s="12">
         <v>15948</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4884,28 +4567,28 @@
         <v>648434063</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C25" s="8">
         <v>149</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G25" s="12">
         <v>17277</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4913,28 +4596,28 @@
         <v>648434062</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C26" s="8">
         <v>149</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G26" s="12">
         <v>18722</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -4942,28 +4625,28 @@
         <v>648434061</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C27" s="8">
         <v>149</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G27" s="12">
         <v>20029</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -4971,28 +4654,28 @@
         <v>648434059</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C28" s="8">
         <v>149</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G28" s="12">
         <v>24794</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -5000,28 +4683,28 @@
         <v>648434058</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C29" s="8">
         <v>149</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G29" s="12">
         <v>26243</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -5029,28 +4712,28 @@
         <v>648434060</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="C30" s="8">
         <v>149</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="G30" s="12">
         <v>22085</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17.100000000000001">
@@ -5058,13 +4741,13 @@
         <v>10198432</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="F31" s="2">
         <v>42254</v>
@@ -5073,10 +4756,10 @@
         <v>25557</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="17.100000000000001">
@@ -5084,25 +4767,25 @@
         <v>10006953</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="G32" s="12">
         <v>122100</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -5113,10 +4796,10 @@
         <v>38</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="F33" s="2">
         <v>42353</v>
@@ -5125,10 +4808,10 @@
         <v>75519</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -5224,1985 +4907,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <pageSetUpPr autoPageBreaks="0"/>
-  </sheetPr>
-  <dimension ref="A1:O59"/>
-  <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
-  <cols>
-    <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="26" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" style="1" customWidth="1"/>
-    <col min="10" max="10" width="46.375" style="1" customWidth="1"/>
-    <col min="11" max="12" width="39" style="1" customWidth="1"/>
-    <col min="13" max="13" width="23.625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="26" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="32.1">
-      <c r="A1" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>350</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>352</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>353</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="32.1">
-      <c r="A2" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18" t="s">
-        <v>357</v>
-      </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="18"/>
-      <c r="N3" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O3" s="18" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="48">
-      <c r="A4" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18" t="s">
-        <v>361</v>
-      </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="O4" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="48">
-      <c r="A5" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O5" s="18" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L6" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O6" s="18" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="272.10000000000002">
-      <c r="A7" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18" t="s">
-        <v>365</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="K7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="M7" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="N7" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O7" s="18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18" t="s">
-        <v>368</v>
-      </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18" t="s">
-        <v>258</v>
-      </c>
-      <c r="K8" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="L8" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O8" s="18" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B9" s="18">
-        <v>251790</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="I9" s="18">
-        <v>918039880000</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>262</v>
-      </c>
-      <c r="K9" s="18">
-        <v>154799</v>
-      </c>
-      <c r="L9" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="18" t="s">
-        <v>369</v>
-      </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18" t="s">
-        <v>370</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18" t="s">
-        <v>371</v>
-      </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18" t="s">
-        <v>372</v>
-      </c>
-      <c r="O10" s="18" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="K11" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L11" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O11" s="18" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="80.099999999999994">
-      <c r="A12" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="K12" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="L12" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="63.95">
-      <c r="A13" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18" t="s">
-        <v>375</v>
-      </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="K13" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O13" s="18" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18" t="s">
-        <v>377</v>
-      </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="K14" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="L14" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O14" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="48">
-      <c r="A15" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18" t="s">
-        <v>124</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="K15" s="18">
-        <v>9611510088</v>
-      </c>
-      <c r="L15" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O15" s="18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="48">
-      <c r="A16" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18" t="s">
-        <v>269</v>
-      </c>
-      <c r="K16" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L16" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O16" s="18" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18" t="s">
-        <v>378</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="K17" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="L17" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="18"/>
-      <c r="N17" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O17" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18" t="s">
-        <v>379</v>
-      </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O18" s="18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
-      <c r="A19" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18" t="s">
-        <v>381</v>
-      </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="L19" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O19" s="18" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
-      <c r="A20" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18" t="s">
-        <v>382</v>
-      </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="K20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="M20" s="18"/>
-      <c r="N20" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="O20" s="18" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
-      <c r="A21" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="K21" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L21" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O21" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="32.1">
-      <c r="A22" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="K22" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L22" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O22" s="18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="32.1">
-      <c r="A23" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="K23" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="O23" s="18" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15">
-      <c r="A24" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="K24" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="L24" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O24" s="18" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18" t="s">
-        <v>388</v>
-      </c>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="K25" s="18" t="s">
-        <v>251</v>
-      </c>
-      <c r="L25" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O25" s="18" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
-      <c r="A26" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L26" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18" t="s">
-        <v>274</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L27" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M27" s="18"/>
-      <c r="N27" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O27" s="18" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
-      <c r="A28" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="K28" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L28" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M28" s="18"/>
-      <c r="N28" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O28" s="18" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="K29" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="L29" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O29" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="32.1">
-      <c r="A30" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="K30" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L30" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M30" s="18"/>
-      <c r="N30" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O30" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18" t="s">
-        <v>389</v>
-      </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="K31" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="O31" s="18" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="48">
-      <c r="A32" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="K32" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="L32" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O32" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="48">
-      <c r="A33" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18" t="s">
-        <v>391</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18" t="s">
-        <v>392</v>
-      </c>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="K33" s="18">
-        <v>200373020</v>
-      </c>
-      <c r="L33" s="18" t="s">
-        <v>393</v>
-      </c>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18" t="s">
-        <v>394</v>
-      </c>
-      <c r="O33" s="18" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18" t="s">
-        <v>395</v>
-      </c>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="K34" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L34" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O34" s="18" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="K35" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L35" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M35" s="18"/>
-      <c r="N35" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O35" s="18" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="K36" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L36" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M36" s="18"/>
-      <c r="N36" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O36" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="96">
-      <c r="A37" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18" t="s">
-        <v>397</v>
-      </c>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18" t="s">
-        <v>177</v>
-      </c>
-      <c r="K37" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="L37" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O37" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
-      <c r="A38" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18" t="s">
-        <v>398</v>
-      </c>
-      <c r="I38" s="18"/>
-      <c r="J38" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="K38" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L38" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M38" s="18"/>
-      <c r="N38" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O38" s="18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
-      <c r="A39" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18" t="s">
-        <v>399</v>
-      </c>
-      <c r="I39" s="18"/>
-      <c r="J39" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="K39" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L39" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M39" s="18"/>
-      <c r="N39" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O39" s="18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15">
-      <c r="A40" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18" t="s">
-        <v>400</v>
-      </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18" t="s">
-        <v>401</v>
-      </c>
-      <c r="I40" s="18"/>
-      <c r="J40" s="18" t="s">
-        <v>402</v>
-      </c>
-      <c r="K40" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L40" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O40" s="18" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="32.1">
-      <c r="A41" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="K41" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L41" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M41" s="18"/>
-      <c r="N41" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O41" s="18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15">
-      <c r="A42" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="K42" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L42" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O42" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15">
-      <c r="A43" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18" t="s">
-        <v>403</v>
-      </c>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="K43" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L43" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O43" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15">
-      <c r="A44" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="K44" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L44" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O44" s="18" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="32.1">
-      <c r="A45" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18" t="s">
-        <v>404</v>
-      </c>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18" t="s">
-        <v>404</v>
-      </c>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="K45" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L45" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="M45" s="18"/>
-      <c r="N45" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="O45" s="18" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="80.099999999999994">
-      <c r="A46" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18" t="s">
-        <v>280</v>
-      </c>
-      <c r="K46" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L46" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="M46" s="18"/>
-      <c r="N46" s="18" t="s">
-        <v>405</v>
-      </c>
-      <c r="O46" s="18" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="A47" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="K47" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L47" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O47" s="18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
-      <c r="A48" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18" t="s">
-        <v>406</v>
-      </c>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="K48" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L48" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M48" s="18"/>
-      <c r="N48" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O48" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="32.1">
-      <c r="A49" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18" t="s">
-        <v>407</v>
-      </c>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="K49" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L49" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O49" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15">
-      <c r="A50" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18" t="s">
-        <v>408</v>
-      </c>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="K50" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L50" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18" t="s">
-        <v>359</v>
-      </c>
-      <c r="O50" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15">
-      <c r="A51" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18" t="s">
-        <v>409</v>
-      </c>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="K51" s="18">
-        <v>9611510088</v>
-      </c>
-      <c r="L51" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M51" s="18"/>
-      <c r="N51" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O51" s="18" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15">
-      <c r="A52" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="K52" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L52" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="M52" s="18"/>
-      <c r="N52" s="18" t="s">
-        <v>360</v>
-      </c>
-      <c r="O52" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15">
-      <c r="A53" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="I53" s="18"/>
-      <c r="J53" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="K53" s="10">
-        <v>100317000000</v>
-      </c>
-      <c r="L53" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="M53" s="18"/>
-      <c r="N53" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="O53" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15">
-      <c r="A54" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18" t="s">
-        <v>411</v>
-      </c>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18" t="s">
-        <v>412</v>
-      </c>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="K54" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="L54" s="18"/>
-      <c r="M54" s="18"/>
-      <c r="N54" s="18">
-        <v>48267</v>
-      </c>
-      <c r="O54" s="18" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15">
-      <c r="A55" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18" t="s">
-        <v>413</v>
-      </c>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="I55" s="18"/>
-      <c r="J55" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K55" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L55" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="O55" s="18" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15">
-      <c r="A56" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B56" s="18"/>
-      <c r="C56" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="18"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18" t="s">
-        <v>415</v>
-      </c>
-      <c r="I56" s="18"/>
-      <c r="J56" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K56" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="L56" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="O56" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18" t="s">
-        <v>416</v>
-      </c>
-      <c r="I57" s="18"/>
-      <c r="J57" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="K57" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L57" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="O57" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15">
-      <c r="A58" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="I58" s="18"/>
-      <c r="J58" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="K58" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="L58" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="O58" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="32.1">
-      <c r="A59" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="I59" s="18"/>
-      <c r="J59" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K59" s="1">
-        <v>9583683</v>
-      </c>
-      <c r="L59" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="O59" s="18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="J1:M54"/>
-  <hyperlinks>
-    <hyperlink ref="K55" r:id="rId1"/>
-    <hyperlink ref="K56" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
@@ -7216,49 +4928,49 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="B1" t="s">
-        <v>417</v>
+        <v>333</v>
       </c>
       <c r="C1" t="s">
-        <v>348</v>
+        <v>334</v>
       </c>
       <c r="D1" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="E1" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>418</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>419</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>419</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>420</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>421</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>422</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>